<commit_message>
-renamed mark code column.
</commit_message>
<xml_diff>
--- a/src/Application/ZMK.Application.Implementation/Templates/commonMarkEventsReportTemplate.xlsx
+++ b/src/Application/ZMK.Application.Implementation/Templates/commonMarkEventsReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrey\source\repos\ZMK\src\Application\ZMK.Application.Implementation\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71210EC8-4543-4527-9DFF-54E32A5144B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5099365E-84F7-46A8-95F0-76F51666EA07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="История марки" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Events">'История марки'!$A$10:$G$11</definedName>
+    <definedName name="Events">'История марки'!$A$11:$G$12</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Дата составления отчета</t>
   </si>
@@ -42,15 +42,9 @@
     <t>{{MarkTitle}}</t>
   </si>
   <si>
-    <t>Код марки</t>
-  </si>
-  <si>
     <t>{{MarkCode}}</t>
   </si>
   <si>
-    <t>Количество марки</t>
-  </si>
-  <si>
     <t>{{MarkCount}}</t>
   </si>
   <si>
@@ -94,6 +88,15 @@
   </si>
   <si>
     <t>{{item.Remark}}</t>
+  </si>
+  <si>
+    <t>Марка</t>
+  </si>
+  <si>
+    <t>Очередность</t>
+  </si>
+  <si>
+    <t>{{MarkOrder}}</t>
   </si>
 </sst>
 </file>
@@ -435,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G10"/>
+  <dimension ref="B2:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,66 +472,74 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="E10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="1" t="s">
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="E11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>